<commit_message>
fix: refine the code
</commit_message>
<xml_diff>
--- a/Data_collection_of_PDB/data/functional site/site classification.xlsx
+++ b/Data_collection_of_PDB/data/functional site/site classification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/PycharmProjects/3D_model/evolution/data/functional site/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065F8753-928F-3A4A-B737-75002DAE447D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC712B0-2D7E-F040-AE7A-F66ABE967F1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13220" yWindow="460" windowWidth="22000" windowHeight="21140" xr2:uid="{71B4A374-86E5-2544-8645-77D1B1AE137E}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t>Secondary structure</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>TURN</t>
-  </si>
-  <si>
-    <t>Complex Interface</t>
   </si>
   <si>
     <t>BINDING</t>
@@ -203,9 +200,6 @@
   </si>
   <si>
     <t>Helix</t>
-  </si>
-  <si>
-    <t>Strand</t>
   </si>
   <si>
     <t>Turn</t>
@@ -350,6 +344,15 @@
   </si>
   <si>
     <t>Non-standard residue</t>
+  </si>
+  <si>
+    <t>Complex_Interface</t>
+  </si>
+  <si>
+    <t>Can't be found from sce</t>
+  </si>
+  <si>
+    <t>Beta strand</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <dimension ref="A1:XFD33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -768,19 +771,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -794,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -809,7 +812,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -824,245 +827,245 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:16384" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
@@ -17447,19 +17450,19 @@
     </row>
     <row r="21" spans="1:16384" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -33843,16 +33846,16 @@
     </row>
     <row r="22" spans="1:16384" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
@@ -50237,16 +50240,16 @@
     </row>
     <row r="23" spans="1:16384" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
@@ -66631,150 +66634,153 @@
     </row>
     <row r="24" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:16384" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>18</v>
+      <c r="D33" s="2" t="s">
+        <v>78</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>